<commit_message>
Backup QR Scanner data - 2025-09-16T04:38:12.965Z - Cache Bust: 1757997492965
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Psychiatry_scanner1757849186950_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
+++ b/log_history/Y4_B2526_Psychiatry_scanner1757849186950_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Psychiatry" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -462,9 +462,1109 @@
         <v>160715@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>221236</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C4" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D4" t="str">
+        <v>14:26:54</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F4" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>221200</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C5" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D5" t="str">
+        <v>14:27:01</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F5" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>221251</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C6" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D6" t="str">
+        <v>14:27:05</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F6" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>221205</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C7" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D7" t="str">
+        <v>14:27:36</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F7" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>221203</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C8" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D8" t="str">
+        <v>14:27:47</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F8" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>221191</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C9" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D9" t="str">
+        <v>14:27:51</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F9" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>221201</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C10" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D10" t="str">
+        <v>14:28:08</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F10" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>221199</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C11" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D11" t="str">
+        <v>14:28:13</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F11" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>221198</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C12" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D12" t="str">
+        <v>14:28:16</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F12" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>221253</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C13" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D13" t="str">
+        <v>14:28:25</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F13" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>221192</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C14" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D14" t="str">
+        <v>14:28:29</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F14" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>221259</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C15" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D15" t="str">
+        <v>14:28:35</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F15" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>221185</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C16" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D16" t="str">
+        <v>14:28:39</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F16" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>221197</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C17" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D17" t="str">
+        <v>14:28:46</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F17" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>221194</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C18" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D18" t="str">
+        <v>14:28:50</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F18" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>221176</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C19" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D19" t="str">
+        <v>14:28:54</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F19" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>221188</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C20" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D20" t="str">
+        <v>14:28:57</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F20" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>221258</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C21" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D21" t="str">
+        <v>14:29:02</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F21" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>221177</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C22" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D22" t="str">
+        <v>14:29:06</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F22" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>221244</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C23" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D23" t="str">
+        <v>14:29:11</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F23" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>221189</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C24" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D24" t="str">
+        <v>14:29:15</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F24" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>221218</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C25" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D25" t="str">
+        <v>14:29:23</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F25" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>221171</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C26" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D26" t="str">
+        <v>14:29:27</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F26" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>221242</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C27" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D27" t="str">
+        <v>14:29:34</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F27" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>221187</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C28" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D28" t="str">
+        <v>14:29:40</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F28" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>221239</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C29" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D29" t="str">
+        <v>14:29:47</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F29" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>221190</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C30" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D30" t="str">
+        <v>14:29:54</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F30" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>221238</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C31" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D31" t="str">
+        <v>14:29:59</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F31" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>221240</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C32" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D32" t="str">
+        <v>14:30:08</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F32" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>221172</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C33" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D33" t="str">
+        <v>14:30:14</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F33" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>221261</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C34" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D34" t="str">
+        <v>14:30:18</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F34" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>221245</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C35" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D35" t="str">
+        <v>14:30:22</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F35" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>221193</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C36" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D36" t="str">
+        <v>14:30:29</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F36" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>221243</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C37" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D37" t="str">
+        <v>14:30:34</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F37" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>221208</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C38" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>14:30:40</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>1321126,410,28/09/2022,null</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C39" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D39" t="str">
+        <v>14:30:45</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>221175</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C40" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D40" t="str">
+        <v>14:30:55</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F40" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>221220</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C41" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D41" t="str">
+        <v>14:31:04</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F41" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>221204</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C42" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>14:31:09</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F42" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>221246</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C43" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D43" t="str">
+        <v>14:31:13</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F43" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>221223</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C44" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D44" t="str">
+        <v>14:31:21</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F44" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>221215</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C45" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D45" t="str">
+        <v>14:31:25</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F45" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>221221</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C46" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D46" t="str">
+        <v>14:31:33</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F46" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>221249</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C47" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D47" t="str">
+        <v>14:31:43</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F47" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>221213</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C48" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D48" t="str">
+        <v>14:31:46</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F48" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>221231</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C49" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D49" t="str">
+        <v>14:31:51</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F49" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>221226</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C50" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D50" t="str">
+        <v>14:31:59</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F50" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>221216</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C51" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D51" t="str">
+        <v>14:32:02</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F51" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>221222</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C52" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D52" t="str">
+        <v>14:32:08</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F52" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>221212</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C53" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D53" t="str">
+        <v>14:32:12</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F53" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>221230</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C54" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D54" t="str">
+        <v>14:32:16</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F54" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>221173</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C55" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D55" t="str">
+        <v>14:32:22</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F55" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>221180</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C56" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D56" t="str">
+        <v>14:32:27</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F56" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>221184</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C57" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D57" t="str">
+        <v>14:32:31</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F57" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>221267</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Psychiatry</v>
+      </c>
+      <c r="C58" t="str">
+        <v>14/09/2025</v>
+      </c>
+      <c r="D58" t="str">
+        <v>14:32:38</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F58" t="str">
+        <v>160715@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F58"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>